<commit_message>
chore: publish document IG 2.0.0
</commit_message>
<xml_diff>
--- a/ig/document/StructureDefinition-medcom-document-homecommunityid-extension.xlsx
+++ b/ig/document/StructureDefinition-medcom-document-homecommunityid-extension.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="159">
   <si>
     <t>Property</t>
   </si>
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.1</t>
+    <t>2.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-12T13:09:34+00:00</t>
+    <t>2026-01-14T10:37:57+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -72,178 +72,181 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>MedCom (http://www.medcom.dk)</t>
+    <t>MedCom (http://www.medcom.dk, fhir@medcom.dk)</t>
   </si>
   <si>
     <t>Jurisdiction</t>
   </si>
   <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Extension containing information about operational and in production home communities (XCA) in Danish Document Sharing</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Copyright</t>
+  </si>
+  <si>
+    <t>FHIR Version</t>
+  </si>
+  <si>
+    <t>4.0.1</t>
+  </si>
+  <si>
+    <t>Kind</t>
+  </si>
+  <si>
+    <t>complex-type</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>Base Definition</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/StructureDefinition/Extension</t>
+  </si>
+  <si>
+    <t>Abstract</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Derivation</t>
+  </si>
+  <si>
+    <t>constraint</t>
+  </si>
+  <si>
+    <t>Context</t>
+  </si>
+  <si>
+    <t>element:Element</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>Slice Name</t>
+  </si>
+  <si>
+    <t>Alias(s)</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Must Support?</t>
+  </si>
+  <si>
+    <t>Is Modifier?</t>
+  </si>
+  <si>
+    <t>Is Summary?</t>
+  </si>
+  <si>
+    <t>Type(s)</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Requirements</t>
+  </si>
+  <si>
+    <t>Default Value</t>
+  </si>
+  <si>
+    <t>Meaning When Missing</t>
+  </si>
+  <si>
+    <t>Fixed Value</t>
+  </si>
+  <si>
+    <t>Pattern</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>Minimum Value</t>
+  </si>
+  <si>
+    <t>Maximum Value</t>
+  </si>
+  <si>
+    <t>Maximum Length</t>
+  </si>
+  <si>
+    <t>Binding Strength</t>
+  </si>
+  <si>
+    <t>Binding Description</t>
+  </si>
+  <si>
+    <t>Binding Value Set</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Slicing Discriminator</t>
+  </si>
+  <si>
+    <t>Slicing Description</t>
+  </si>
+  <si>
+    <t>Slicing Ordered</t>
+  </si>
+  <si>
+    <t>Slicing Rules</t>
+  </si>
+  <si>
+    <t>Base Path</t>
+  </si>
+  <si>
+    <t>Base Min</t>
+  </si>
+  <si>
+    <t>Base Max</t>
+  </si>
+  <si>
+    <t>Condition(s)</t>
+  </si>
+  <si>
+    <t>Constraint(s)</t>
+  </si>
+  <si>
+    <t>Mapping: RIM Mapping</t>
+  </si>
+  <si>
     <t/>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Extension containing information about operational and in production home communities (XCA) in Danish Document Sharing</t>
-  </si>
-  <si>
-    <t>Purpose</t>
-  </si>
-  <si>
-    <t>Copyright</t>
-  </si>
-  <si>
-    <t>FHIR Version</t>
-  </si>
-  <si>
-    <t>4.0.1</t>
-  </si>
-  <si>
-    <t>Kind</t>
-  </si>
-  <si>
-    <t>complex-type</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Extension</t>
-  </si>
-  <si>
-    <t>Base Definition</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/StructureDefinition/Extension</t>
-  </si>
-  <si>
-    <t>Abstract</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>Derivation</t>
-  </si>
-  <si>
-    <t>constraint</t>
-  </si>
-  <si>
-    <t>Context</t>
-  </si>
-  <si>
-    <t>element:Element</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Path</t>
-  </si>
-  <si>
-    <t>Slice Name</t>
-  </si>
-  <si>
-    <t>Alias(s)</t>
-  </si>
-  <si>
-    <t>Label</t>
-  </si>
-  <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Must Support?</t>
-  </si>
-  <si>
-    <t>Is Modifier?</t>
-  </si>
-  <si>
-    <t>Is Summary?</t>
-  </si>
-  <si>
-    <t>Type(s)</t>
-  </si>
-  <si>
-    <t>Short</t>
-  </si>
-  <si>
-    <t>Definition</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Requirements</t>
-  </si>
-  <si>
-    <t>Default Value</t>
-  </si>
-  <si>
-    <t>Meaning When Missing</t>
-  </si>
-  <si>
-    <t>Fixed Value</t>
-  </si>
-  <si>
-    <t>Pattern</t>
-  </si>
-  <si>
-    <t>Example</t>
-  </si>
-  <si>
-    <t>Minimum Value</t>
-  </si>
-  <si>
-    <t>Maximum Value</t>
-  </si>
-  <si>
-    <t>Maximum Length</t>
-  </si>
-  <si>
-    <t>Binding Strength</t>
-  </si>
-  <si>
-    <t>Binding Description</t>
-  </si>
-  <si>
-    <t>Binding Value Set</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Slicing Discriminator</t>
-  </si>
-  <si>
-    <t>Slicing Description</t>
-  </si>
-  <si>
-    <t>Slicing Ordered</t>
-  </si>
-  <si>
-    <t>Slicing Rules</t>
-  </si>
-  <si>
-    <t>Base Path</t>
-  </si>
-  <si>
-    <t>Base Min</t>
-  </si>
-  <si>
-    <t>Base Max</t>
-  </si>
-  <si>
-    <t>Condition(s)</t>
-  </si>
-  <si>
-    <t>Constraint(s)</t>
-  </si>
-  <si>
-    <t>Mapping: RIM Mapping</t>
   </si>
   <si>
     <t>0</t>
@@ -999,26 +1002,26 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="J2" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="K2" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L2" t="s" s="2">
         <v>9</v>
@@ -1029,1322 +1032,1322 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="S2" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="T2" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="U2" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="V2" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="W2" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="X2" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Y2" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Z2" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AA2" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AB2" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AC2" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AD2" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AE2" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AF2" t="s" s="2">
         <v>30</v>
       </c>
       <c r="AG2" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AH2" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AI2" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AJ2" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AK2" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="J3" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="K3" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M3" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="S3" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="T3" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="U3" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="V3" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="W3" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="X3" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Y3" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Z3" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AA3" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AB3" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AC3" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AD3" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AE3" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AF3" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AG3" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AH3" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AI3" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AJ3" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AK3" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" hidden="true">
       <c r="A4" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H4" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="I4" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L4" t="s" s="2">
         <v>30</v>
       </c>
       <c r="M4" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Q4" s="2"/>
       <c r="R4" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="S4" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="T4" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="U4" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="V4" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="W4" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="X4" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Y4" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Z4" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AA4" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AB4" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AC4" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AD4" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AE4" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AF4" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AG4" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AH4" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AK4" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H5" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="I5" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="N5" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="O5" s="2"/>
       <c r="P5" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Q5" s="2"/>
       <c r="R5" t="s" s="2">
         <v>3</v>
       </c>
       <c r="S5" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="T5" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="U5" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="V5" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="W5" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="X5" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Y5" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Z5" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AA5" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AB5" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AC5" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AD5" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AG5" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AH5" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AK5" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H6" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="I6" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Q6" s="2"/>
       <c r="R6" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="S6" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="T6" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="U6" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="V6" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="W6" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Y6" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Z6" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AA6" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AB6" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AC6" s="2"/>
       <c r="AD6" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AF6" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AG6" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AH6" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AI6" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ6" t="s" s="2">
+        <v>108</v>
+      </c>
+      <c r="AK6" t="s" s="2">
         <v>101</v>
-      </c>
-      <c r="AG6" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AH6" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AI6" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ6" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="AK6" t="s" s="2">
-        <v>100</v>
       </c>
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G7" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H7" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I7" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="J7" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="M7" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="S7" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="T7" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="U7" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="V7" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="W7" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="X7" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Y7" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Z7" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AA7" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AB7" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AC7" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AD7" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AE7" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AF7" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AG7" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AH7" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AI7" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AJ7" t="s" s="2">
+        <v>108</v>
+      </c>
+      <c r="AK7" t="s" s="2">
         <v>101</v>
-      </c>
-      <c r="AG7" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AH7" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AI7" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="AJ7" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="AK7" t="s" s="2">
-        <v>100</v>
       </c>
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G8" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H8" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="I8" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="S8" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="T8" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="U8" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="V8" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="W8" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="X8" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Y8" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Z8" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AA8" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AB8" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AC8" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AD8" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AF8" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AG8" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AH8" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AI8" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AJ8" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AK8" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G9" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H9" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="I9" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="M9" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N9" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Q9" s="2"/>
       <c r="R9" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="S9" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="T9" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="U9" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="V9" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="W9" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="X9" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Y9" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Z9" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AA9" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AB9" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AC9" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AD9" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AF9" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AG9" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AH9" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AK9" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I10" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N10" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="O10" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="P10" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Q10" s="2"/>
       <c r="R10" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="S10" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="T10" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="U10" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="V10" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="W10" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="X10" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Y10" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Z10" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AA10" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AB10" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AC10" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AD10" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AF10" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AG10" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AH10" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AK10" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="I11" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="N11" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="O11" s="2"/>
       <c r="P11" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Q11" s="2"/>
       <c r="R11" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="S11" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="T11" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="U11" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="V11" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="W11" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="X11" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Y11" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Z11" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AA11" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AB11" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AC11" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AD11" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AF11" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AG11" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AH11" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AK11" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H12" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I12" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="P12" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Q12" s="2"/>
       <c r="R12" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="S12" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="T12" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="U12" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="V12" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="W12" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="X12" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Y12" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Z12" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AA12" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AB12" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AC12" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AD12" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AG12" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AH12" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H13" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="I13" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="P13" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Q13" s="2"/>
       <c r="R13" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="S13" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="T13" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="U13" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="V13" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="W13" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="X13" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Y13" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Z13" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AA13" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AB13" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AC13" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AD13" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AG13" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AH13" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H14" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="I14" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="N14" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="O14" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="P14" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Q14" s="2"/>
       <c r="R14" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="S14" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="T14" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="U14" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="V14" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="W14" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Y14" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="Z14" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AA14" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AB14" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AC14" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AD14" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="AG14" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AH14" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AI14" t="s" s="2">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>